<commit_message>
I hope excel exportation is fully completed
</commit_message>
<xml_diff>
--- a/templates/excel/Archive.xlsx
+++ b/templates/excel/Archive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\algop\Desktop\SerWibe\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DF072A-2EEE-43F1-A35B-A2EFF2EB59CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB36291D-BCEA-4F18-9857-3FACE1B1A23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{DC48A8AF-A767-4AA2-A5D2-407EE1799F05}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>№</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>ИД</t>
+  </si>
+  <si>
+    <t>Тан нархи</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -655,35 +658,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FDFA5E-B4CB-4582-923B-77DCCF787F83}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.109375" style="7" customWidth="1"/>
     <col min="2" max="2" width="21.88671875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="7" customWidth="1"/>
+    <col min="3" max="5" width="19.21875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>